<commit_message>
summary: 6. CONSULTA LIBRERIA PYTHON
</commit_message>
<xml_diff>
--- a/6. CONSULTA LIBRERIA PYTHON/BDEstudiantes.xlsx
+++ b/6. CONSULTA LIBRERIA PYTHON/BDEstudiantes.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correouisedu-my.sharepoint.com/personal/laura2220100_correo_uis_edu_co/Documents/Documents/GitHub/EdD-AdA/6. CONSULTA LIBRERIA PYTHON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{78DF31DB-A57E-4BA2-BF05-0AB27ED1E448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B369FCB-DCEC-430F-8283-C8BE94D9E4E3}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{78DF31DB-A57E-4BA2-BF05-0AB27ED1E448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8431973-D84D-45FE-98CA-A211616E540E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E14E0F82-DB24-4F28-B67E-22A59E5901DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$6501</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19908,15 +19911,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -19938,10 +19938,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20243,8 +20239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B48BC4B-59F6-40D4-8257-4C2173B355DE}">
   <dimension ref="A1:F6501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20261,7 +20257,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -20305,7 +20301,7 @@
       <c r="B5" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -20330,7 +20326,7 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -91767,6 +91763,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C6501" xr:uid="{0B48BC4B-59F6-40D4-8257-4C2173B355DE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>